<commit_message>
Basic APACHE POI Programs
</commit_message>
<xml_diff>
--- a/target/classes/TestData/cities1.xlsx
+++ b/target/classes/TestData/cities1.xlsx
@@ -12,7 +12,35 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>EmpID</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>200000</t>
+  </si>
+  <si>
+    <t>Suresh</t>
+  </si>
+  <si>
+    <t>244000</t>
+  </si>
+  <si>
+    <t>Mahesh</t>
+  </si>
+  <si>
+    <t>203000</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -62,28 +90,48 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1"/>
-      <c r="B1"/>
-      <c r="C1"/>
-      <c r="D1"/>
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2"/>
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
+      <c r="A2" t="n">
+        <v>101.0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3"/>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
+      <c r="A3" t="n">
+        <v>101.0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4"/>
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
+      <c r="A4" t="n">
+        <v>101.0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>